<commit_message>
Refactor api methods, getters and setters. Construir remision y factura en unico método.
</commit_message>
<xml_diff>
--- a/Libro1 - copia.xlsx
+++ b/Libro1 - copia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marif\Desktop\alegraApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49426132-B5F8-4160-8B18-97763693A943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DC7C2F-ECBB-4437-984F-1FB548DB3B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FAD0E68C-6DCF-4695-A4DE-AD78308D2F78}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>Navaja pico de loro gde</t>
   </si>
@@ -94,15 +94,6 @@
     <t>NOTAS</t>
   </si>
   <si>
-    <t>Empacó</t>
-  </si>
-  <si>
-    <t>#Paquetes</t>
-  </si>
-  <si>
-    <t>Guía</t>
-  </si>
-  <si>
     <t>Transportadora</t>
   </si>
   <si>
@@ -157,10 +148,19 @@
     <t>FE2610</t>
   </si>
   <si>
-    <t># paq</t>
-  </si>
-  <si>
     <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t>Guia</t>
+  </si>
+  <si>
+    <t>NumeroPaquetes</t>
+  </si>
+  <si>
+    <t>FechaVencimiento</t>
+  </si>
+  <si>
+    <t>Empaco</t>
   </si>
 </sst>
 </file>
@@ -172,7 +172,7 @@
     <numFmt numFmtId="165" formatCode="d/m/yy"/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +207,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -271,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -379,6 +387,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -697,71 +708,71 @@
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>28</v>
+        <v>34</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>26</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G1" s="28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H1" s="28" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I1" s="28" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J1" s="28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="O1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="P1" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="Q1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="28" t="s">
+      <c r="R1" s="28" t="s">
         <v>14</v>
-      </c>
-      <c r="R1" s="28" t="s">
-        <v>40</v>
       </c>
       <c r="S1" s="28" t="s">
         <v>13</v>
@@ -778,32 +789,32 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B2" s="27"/>
       <c r="C2" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="7"/>
+        <v>37</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="25"/>
       <c r="H2" s="7"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="23"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="5"/>
       <c r="L2" s="23"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="21"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="22"/>
       <c r="R2" s="21"/>
       <c r="S2" s="20"/>
       <c r="T2" s="19"/>
@@ -814,55 +825,57 @@
       <c r="A3" s="17">
         <v>44366</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="17">
+        <v>44366</v>
+      </c>
+      <c r="C3" s="13">
         <v>6</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="D3" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="15">
-        <v>31245</v>
-      </c>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="18"/>
+      <c r="G3" s="15">
+        <v>8104442</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="31">
+      <c r="K3" s="31">
         <v>14228</v>
       </c>
-      <c r="K3" s="11">
+      <c r="L3" s="11">
         <v>1</v>
       </c>
-      <c r="L3" s="38" t="s">
+      <c r="M3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="N3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="32">
+      <c r="O3" s="32">
         <v>208</v>
       </c>
-      <c r="O3" s="42" t="s">
+      <c r="P3" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="10">
+      <c r="Q3" s="10">
         <v>180</v>
       </c>
-      <c r="Q3" s="9">
+      <c r="R3" s="9">
         <v>1791</v>
       </c>
-      <c r="R3" s="9"/>
       <c r="S3" s="37">
-        <f>P3*Q3</f>
+        <f>Q3*R3</f>
         <v>322380</v>
       </c>
       <c r="T3" s="9">
@@ -873,41 +886,41 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="17"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13" t="s">
-        <v>41</v>
-      </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="13"/>
       <c r="D4" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="16"/>
+      <c r="G4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="11"/>
+      <c r="H4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="13"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="14"/>
       <c r="L4" s="11"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="32">
+      <c r="M4" s="11"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="32">
         <v>698</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="P4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="P4" s="10">
+      <c r="Q4" s="10">
         <v>30</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="R4" s="9">
         <v>15661.59</v>
       </c>
-      <c r="R4" s="9"/>
       <c r="S4" s="9">
-        <f>P4*Q4</f>
+        <f>Q4*R4</f>
         <v>469847.7</v>
       </c>
       <c r="T4" s="9">
@@ -918,35 +931,35 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="17"/>
-      <c r="B5" s="13"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="15" t="s">
+      <c r="E5" s="13"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="13"/>
       <c r="H5" s="13"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="11"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="14"/>
       <c r="L5" s="11"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="32">
+      <c r="M5" s="11"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="32">
         <v>1220</v>
       </c>
-      <c r="O5" s="43" t="s">
+      <c r="P5" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="P5" s="10">
+      <c r="Q5" s="10">
         <v>24</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="R5" s="9">
         <v>9376.01</v>
       </c>
-      <c r="R5" s="9"/>
       <c r="S5" s="9">
-        <f>P5*Q5</f>
+        <f>Q5*R5</f>
         <v>225024.24</v>
       </c>
       <c r="T5" s="9">
@@ -957,22 +970,22 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="5"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="5"/>
       <c r="P6" s="2"/>
-      <c r="Q6" s="3"/>
+      <c r="Q6" s="2"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
       <c r="T6" s="4"/>
@@ -983,56 +996,58 @@
       <c r="A7" s="17">
         <v>44365</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="17">
+        <v>44365</v>
+      </c>
+      <c r="C7" s="13">
         <v>30</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="D7" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0.19</v>
+      </c>
+      <c r="G7" s="33">
+        <v>8104442</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="40">
+        <v>15751</v>
+      </c>
+      <c r="L7" s="11">
+        <v>1</v>
+      </c>
+      <c r="M7" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" s="13"/>
+      <c r="O7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="16">
-        <v>0.19</v>
-      </c>
-      <c r="F7" s="33" t="s">
+      <c r="P7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" s="40">
-        <v>15751</v>
-      </c>
-      <c r="K7" s="11">
-        <v>1</v>
-      </c>
-      <c r="L7" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="M7" s="13"/>
-      <c r="N7" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="O7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="P7" s="10">
+      <c r="Q7" s="10">
         <v>204</v>
       </c>
-      <c r="Q7" s="9">
-        <f>IF(E7="",U7, ROUND(U7/(1+E7),0))</f>
+      <c r="R7" s="9">
+        <f>IF(F7="",U7, ROUND(U7/(1+F7),0))</f>
         <v>1280</v>
       </c>
-      <c r="R7" s="9"/>
       <c r="S7" s="9">
-        <f>P7*Q7</f>
+        <f>Q7*R7</f>
         <v>261120</v>
       </c>
       <c r="T7" s="9">
@@ -1045,38 +1060,38 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="30"/>
-      <c r="B8" s="13"/>
+      <c r="B8" s="30"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="16">
+      <c r="E8" s="13"/>
+      <c r="F8" s="16">
         <v>0.19</v>
       </c>
-      <c r="F8" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="30"/>
+      <c r="G8" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="H8" s="30"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="11"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="14"/>
       <c r="L8" s="11"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="O8" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="P8" s="10">
+      <c r="M8" s="11"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q8" s="10">
         <v>2</v>
       </c>
-      <c r="Q8" s="36">
-        <f>IF(E8="",U8, ROUND(U8/(1+E8),0))</f>
+      <c r="R8" s="36">
+        <f>IF(F8="",U8, ROUND(U8/(1+F8),0))</f>
         <v>37734</v>
       </c>
-      <c r="R8" s="9"/>
       <c r="S8" s="9">
-        <f>P8*Q8</f>
+        <f>Q8*R8</f>
         <v>75468</v>
       </c>
       <c r="T8" s="9">
@@ -1092,19 +1107,19 @@
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="5"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="5"/>
       <c r="P9" s="2"/>
-      <c r="Q9" s="3"/>
+      <c r="Q9" s="2"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="4"/>
@@ -1115,56 +1130,58 @@
       <c r="A10" s="17">
         <v>44365</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="17">
+        <v>44365</v>
+      </c>
+      <c r="C10" s="13">
         <v>30</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="D10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="16">
+        <v>0.19</v>
+      </c>
+      <c r="G10" s="33">
+        <v>8104441</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="40">
+        <v>15751</v>
+      </c>
+      <c r="L10" s="11">
+        <v>1</v>
+      </c>
+      <c r="M10" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10" s="13"/>
+      <c r="O10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="16">
-        <v>0.19</v>
-      </c>
-      <c r="F10" s="33" t="s">
+      <c r="P10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="40">
-        <v>15751</v>
-      </c>
-      <c r="K10" s="11">
-        <v>1</v>
-      </c>
-      <c r="L10" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="M10" s="13"/>
-      <c r="N10" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="O10" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="P10" s="10">
+      <c r="Q10" s="10">
         <v>204</v>
       </c>
-      <c r="Q10" s="9">
-        <f>IF(E10="",U10, ROUND(U10/(1+E10),0))</f>
+      <c r="R10" s="9">
+        <f>IF(F10="",U10, ROUND(U10/(1+F10),0))</f>
         <v>1280</v>
       </c>
-      <c r="R10" s="9"/>
       <c r="S10" s="9">
-        <f>P10*Q10</f>
+        <f>Q10*R10</f>
         <v>261120</v>
       </c>
       <c r="T10" s="9">

</xml_diff>

<commit_message>
Se separa logica de Api, se eliminan métodos sin utilizar del modelo, se pasa metodo leer terminos y condiciones a utils.
</commit_message>
<xml_diff>
--- a/Libro1 - copia.xlsx
+++ b/Libro1 - copia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marif\Desktop\alegraApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DC7C2F-ECBB-4437-984F-1FB548DB3B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4F4AF3-3F10-48C9-8DE8-37E3AE6832F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FAD0E68C-6DCF-4695-A4DE-AD78308D2F78}"/>
   </bookViews>
@@ -708,7 +708,7 @@
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Tolerancia a fallos con getIdCliente.
</commit_message>
<xml_diff>
--- a/Libro1 - copia.xlsx
+++ b/Libro1 - copia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marif\Desktop\alegraApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4F4AF3-3F10-48C9-8DE8-37E3AE6832F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EAC5DF-E0F4-4BE3-A125-283243052DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FAD0E68C-6DCF-4695-A4DE-AD78308D2F78}"/>
   </bookViews>
@@ -279,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -390,6 +390,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -708,7 +711,7 @@
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,7 +842,7 @@
       </c>
       <c r="F3" s="18"/>
       <c r="G3" s="15">
-        <v>8104442</v>
+        <v>8104448</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>7</v>
@@ -996,7 +999,7 @@
       <c r="A7" s="17">
         <v>44365</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="45">
         <v>44365</v>
       </c>
       <c r="C7" s="13">

</xml_diff>

<commit_message>
Tolerancia a fallos por getProductId. Mensajes de informacion.
</commit_message>
<xml_diff>
--- a/Libro1 - copia.xlsx
+++ b/Libro1 - copia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marif\Desktop\alegraApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EAC5DF-E0F4-4BE3-A125-283243052DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1C7DE1-E78E-4958-B17C-C4247830B4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FAD0E68C-6DCF-4695-A4DE-AD78308D2F78}"/>
   </bookViews>
@@ -711,7 +711,7 @@
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,7 +842,7 @@
       </c>
       <c r="F3" s="18"/>
       <c r="G3" s="15">
-        <v>8104448</v>
+        <v>8104441</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Iva 5%, ref y id como int, Excel nuevo formato.
</commit_message>
<xml_diff>
--- a/Libro1 - copia.xlsx
+++ b/Libro1 - copia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marif\Desktop\alegraApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3CAE6A-E7F7-4704-8F65-6BEDCA69ADE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941D2656-0218-442A-8B8D-354C9F48B67C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FAD0E68C-6DCF-4695-A4DE-AD78308D2F78}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FAD0E68C-6DCF-4695-A4DE-AD78308D2F78}"/>
   </bookViews>
   <sheets>
     <sheet name="ENVIABLES" sheetId="1" r:id="rId1"/>
@@ -35,16 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
-  <si>
-    <t>Navaja pico de loro gde</t>
-  </si>
-  <si>
-    <t>Poliester 4h 1 Kg</t>
-  </si>
-  <si>
-    <t>Fibra pp 12000 200 gr surtida</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>5 pacas</t>
   </si>
@@ -109,18 +100,9 @@
     <t>FORMA DE PAGO</t>
   </si>
   <si>
-    <t>Estella González Arias</t>
-  </si>
-  <si>
     <t>Tuluá</t>
   </si>
   <si>
-    <t>Soga cabuya 1/2 13mm 204m</t>
-  </si>
-  <si>
-    <t>Fibra pp 18000 5 kg negra</t>
-  </si>
-  <si>
     <t>FECHA</t>
   </si>
   <si>
@@ -151,12 +133,6 @@
     <t>ClienteNombre</t>
   </si>
   <si>
-    <t>Jorge</t>
-  </si>
-  <si>
-    <t>Arley Jose Varon</t>
-  </si>
-  <si>
     <t>Factura</t>
   </si>
   <si>
@@ -164,6 +140,24 @@
   </si>
   <si>
     <t>FACT/REMIS</t>
+  </si>
+  <si>
+    <t>Patricia rendon</t>
+  </si>
+  <si>
+    <t>Samuel rendon</t>
+  </si>
+  <si>
+    <t>Samuel Rendon SAS</t>
+  </si>
+  <si>
+    <t>Fibra 12000</t>
+  </si>
+  <si>
+    <t>Herradura</t>
+  </si>
+  <si>
+    <t>Cabuya</t>
   </si>
 </sst>
 </file>
@@ -175,7 +169,7 @@
     <numFmt numFmtId="165" formatCode="d/m/yy"/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +207,20 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -282,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -307,9 +315,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -332,12 +337,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -347,27 +346,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -379,9 +366,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -392,6 +376,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -708,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBDEF7A-7AF5-4F3E-81D7-89F968F33B79}">
-  <dimension ref="A1:X10"/>
+  <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -725,198 +736,206 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="C1" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="27" t="s">
+      <c r="E1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="F1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="G1" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="O1" s="27" t="s">
+      <c r="I1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="J1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="27" t="s">
+      <c r="K1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="27" t="s">
+      <c r="L1" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="27" t="s">
+      <c r="P1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="Q1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="R1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="S1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="W1" s="27" t="s">
+      <c r="T1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="X1" s="43" t="s">
-        <v>36</v>
+      <c r="U1" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="V1" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="W1" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="X1" s="35" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A2" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="26"/>
+      <c r="A2" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="23"/>
       <c r="C2" s="7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="24"/>
+        <v>25</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="22"/>
+      <c r="H2" s="43"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="22"/>
+      <c r="K2" s="21"/>
       <c r="L2" s="5"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
       <c r="O2" s="7"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="18"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="17"/>
       <c r="V2" s="2"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A3" s="16">
+      <c r="A3" s="15">
         <v>44366</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="15">
         <v>44366</v>
       </c>
       <c r="C3" s="12">
         <v>6</v>
       </c>
-      <c r="D3" s="38" t="s">
-        <v>41</v>
+      <c r="D3" s="31" t="s">
+        <v>32</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="14">
-        <v>8104441</v>
+        <v>4</v>
+      </c>
+      <c r="F3" s="16">
+        <v>0.19</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="44">
+        <v>39456079</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="L3" s="30">
+        <v>2</v>
+      </c>
+      <c r="L3" s="26">
         <v>14228</v>
       </c>
       <c r="M3" s="11">
         <v>1</v>
       </c>
-      <c r="N3" s="37" t="s">
-        <v>4</v>
+      <c r="N3" s="30" t="s">
+        <v>1</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="P3" s="31">
-        <v>208</v>
-      </c>
-      <c r="Q3" s="41" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="P3" s="41">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="33" t="s">
+        <v>38</v>
       </c>
       <c r="R3" s="10">
-        <v>180</v>
+        <v>320</v>
       </c>
       <c r="S3" s="9">
-        <v>1791</v>
-      </c>
-      <c r="T3" s="36">
+        <v>11000</v>
+      </c>
+      <c r="T3" s="29">
         <f>R3*S3</f>
-        <v>322380</v>
+        <v>3520000</v>
       </c>
       <c r="U3" s="9">
         <v>36</v>
       </c>
-      <c r="V3" s="9"/>
+      <c r="V3" s="9">
+        <f>S3*(1+F3)</f>
+        <v>13090</v>
+      </c>
       <c r="W3" s="8">
-        <f>S3*R3</f>
-        <v>322380</v>
+        <f>V3*R3</f>
+        <v>4188800</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="F4" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="45"/>
       <c r="I4" s="12" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="11"/>
@@ -924,40 +943,45 @@
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
       <c r="O4" s="12"/>
-      <c r="P4" s="31">
-        <v>698</v>
+      <c r="P4" s="41">
+        <v>2</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="R4" s="10">
         <v>30</v>
       </c>
       <c r="S4" s="9">
-        <v>15662</v>
+        <v>12000</v>
       </c>
       <c r="T4" s="9">
         <f>R4*S4</f>
-        <v>469860</v>
+        <v>360000</v>
       </c>
       <c r="U4" s="9">
         <v>30</v>
       </c>
-      <c r="V4" s="9"/>
+      <c r="V4" s="9">
+        <f t="shared" ref="V4:V5" si="0">S4*(1+F4)</f>
+        <v>12600</v>
+      </c>
       <c r="W4" s="8">
-        <f t="shared" ref="W4:W5" si="0">S4*R4</f>
-        <v>469860</v>
+        <f>V4*R4</f>
+        <v>378000</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="14"/>
+      <c r="F5" s="14">
+        <v>0</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="46"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="11"/>
@@ -965,29 +989,32 @@
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
       <c r="O5" s="12"/>
-      <c r="P5" s="31">
-        <v>1220</v>
-      </c>
-      <c r="Q5" s="42" t="s">
-        <v>0</v>
+      <c r="P5" s="41">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="34" t="s">
+        <v>40</v>
       </c>
       <c r="R5" s="10">
         <v>24</v>
       </c>
       <c r="S5" s="9">
-        <v>9376</v>
+        <v>3000</v>
       </c>
       <c r="T5" s="9">
         <f>R5*S5</f>
-        <v>225024</v>
+        <v>72000</v>
       </c>
       <c r="U5" s="9">
         <v>2.76</v>
       </c>
-      <c r="V5" s="9"/>
+      <c r="V5" s="9">
+        <f t="shared" si="0"/>
+        <v>3000</v>
+      </c>
       <c r="W5" s="8">
-        <f t="shared" si="0"/>
-        <v>225024</v>
+        <f t="shared" ref="W5:W7" si="1">V5*R5</f>
+        <v>72000</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.35">
@@ -998,7 +1025,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="2"/>
+      <c r="H6" s="42"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -1006,132 +1033,128 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-      <c r="P6" s="5"/>
+      <c r="P6" s="42"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
       <c r="U6" s="4"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="1"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
       <c r="X6" s="1"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A7" s="16">
+      <c r="A7" s="15">
         <v>44365</v>
       </c>
-      <c r="B7" s="44">
+      <c r="B7" s="36">
         <v>44365</v>
       </c>
       <c r="C7" s="12">
         <v>30</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="15">
-        <v>0.19</v>
-      </c>
-      <c r="G7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="47">
+        <v>3560832</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="32">
-        <v>8104442</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>30</v>
-      </c>
       <c r="K7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="L7" s="39">
+        <v>2</v>
+      </c>
+      <c r="L7" s="32">
         <v>15751</v>
       </c>
       <c r="M7" s="11">
         <v>1</v>
       </c>
-      <c r="N7" s="33" t="s">
-        <v>4</v>
+      <c r="N7" s="27" t="s">
+        <v>1</v>
       </c>
       <c r="O7" s="12"/>
-      <c r="P7" s="31">
-        <v>957</v>
-      </c>
-      <c r="Q7" s="42" t="s">
-        <v>26</v>
+      <c r="P7" s="41">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="33" t="s">
+        <v>38</v>
       </c>
       <c r="R7" s="10">
-        <v>204</v>
+        <v>320</v>
       </c>
       <c r="S7" s="9">
-        <f>IF(F7="",V7, ROUND(V7/(1+F7),0))</f>
-        <v>1280</v>
-      </c>
-      <c r="T7" s="9">
+        <v>11000</v>
+      </c>
+      <c r="T7" s="29">
         <f>R7*S7</f>
-        <v>261120</v>
+        <v>3520000</v>
       </c>
       <c r="U7" s="9">
-        <v>25</v>
-      </c>
-      <c r="V7" s="40">
-        <v>1523.2</v>
+        <v>36</v>
+      </c>
+      <c r="V7" s="9">
+        <f>S7*(1+F7)</f>
+        <v>11000</v>
       </c>
       <c r="W7" s="8">
-        <f>R7*S7*(1+F7)</f>
-        <v>310732.79999999999</v>
+        <f t="shared" si="1"/>
+        <v>3520000</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
-      <c r="F8" s="15">
-        <v>0.19</v>
-      </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
       <c r="K8" s="11"/>
       <c r="L8" s="13"/>
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
       <c r="O8" s="12"/>
-      <c r="P8" s="31">
-        <v>631</v>
-      </c>
-      <c r="Q8" s="42" t="s">
-        <v>27</v>
+      <c r="P8" s="41">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="R8" s="10">
-        <v>2</v>
-      </c>
-      <c r="S8" s="35">
-        <f>IF(F8="",V8, ROUND(V8/(1+F8),0))</f>
-        <v>37734</v>
+        <v>30</v>
+      </c>
+      <c r="S8" s="9">
+        <v>12000</v>
       </c>
       <c r="T8" s="9">
         <f>R8*S8</f>
-        <v>75468</v>
+        <v>360000</v>
       </c>
       <c r="U8" s="9">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="V8" s="9">
-        <v>44903.46</v>
+        <f t="shared" ref="V8" si="2">S8*(1+F8)</f>
+        <v>12000</v>
       </c>
       <c r="W8" s="8">
-        <f>R8*S8*(1+F8)</f>
-        <v>89806.92</v>
+        <f>V8*R8</f>
+        <v>360000</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.35">
@@ -1142,7 +1165,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="42"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -1150,87 +1173,90 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
-      <c r="P9" s="5"/>
+      <c r="P9" s="42"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
       <c r="U9" s="4"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
       <c r="X9" s="1"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A10" s="16">
+      <c r="A10" s="15">
         <v>44365</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="15">
         <v>44365</v>
       </c>
       <c r="C10" s="12">
         <v>30</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="15">
+        <v>4</v>
+      </c>
+      <c r="F10" s="14">
         <v>0.19</v>
       </c>
-      <c r="G10" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="32">
-        <v>8104441</v>
+      <c r="G10" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="47">
+        <v>901352563</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="L10" s="39">
+        <v>2</v>
+      </c>
+      <c r="L10" s="32">
         <v>15751</v>
       </c>
       <c r="M10" s="11">
         <v>1</v>
       </c>
-      <c r="N10" s="33" t="s">
-        <v>4</v>
+      <c r="N10" s="27" t="s">
+        <v>1</v>
       </c>
       <c r="O10" s="12"/>
-      <c r="P10" s="31">
-        <v>957</v>
-      </c>
-      <c r="Q10" s="42" t="s">
-        <v>26</v>
+      <c r="P10" s="41">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="34" t="s">
+        <v>40</v>
       </c>
       <c r="R10" s="10">
-        <v>204</v>
+        <v>24</v>
       </c>
       <c r="S10" s="9">
-        <f>IF(F10="",V10, ROUND(V10/(1+F10),0))</f>
-        <v>1280</v>
+        <v>3000</v>
       </c>
       <c r="T10" s="9">
         <f>R10*S10</f>
-        <v>261120</v>
+        <v>72000</v>
       </c>
       <c r="U10" s="9">
-        <v>25</v>
-      </c>
-      <c r="V10" s="40">
-        <v>1523.2</v>
+        <v>2.76</v>
+      </c>
+      <c r="V10" s="9">
+        <f t="shared" ref="V10" si="3">S10*(1+F10)</f>
+        <v>3570</v>
       </c>
       <c r="W10" s="8">
-        <f t="shared" ref="W10" si="1">R10*S10*(1+F10)</f>
-        <v>310732.79999999999</v>
-      </c>
+        <f>V10*R10</f>
+        <v>85680</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="H14" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Leer Pendientes, convención snake_case.
</commit_message>
<xml_diff>
--- a/Libro1 - copia.xlsx
+++ b/Libro1 - copia.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marif\Desktop\alegraApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941D2656-0218-442A-8B8D-354C9F48B67C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DC78AF-3E22-4FA4-A6BD-67DC1BE4E6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FAD0E68C-6DCF-4695-A4DE-AD78308D2F78}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>5 pacas</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>Cabuya</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <t>Cargado</t>
   </si>
 </sst>
 </file>
@@ -721,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBDEF7A-7AF5-4F3E-81D7-89F968F33B79}">
   <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -918,6 +924,9 @@
         <f>V3*R3</f>
         <v>4188800</v>
       </c>
+      <c r="X3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="15"/>
@@ -937,7 +946,6 @@
       <c r="I4" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="12"/>
       <c r="K4" s="11"/>
       <c r="L4" s="13"/>
       <c r="M4" s="11"/>
@@ -1109,8 +1117,11 @@
         <v>11000</v>
       </c>
       <c r="W7" s="8">
-        <f t="shared" si="1"/>
+        <f>V7*R7</f>
         <v>3520000</v>
+      </c>
+      <c r="X7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.35">
@@ -1254,6 +1265,9 @@
         <f>V10*R10</f>
         <v>85680</v>
       </c>
+      <c r="X10" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="H14" s="38"/>

</xml_diff>